<commit_message>
Added 4 more modes which use _mm_pause() instead of sleep(). I add them to both linked list and ring buffer, tested them and add/updated the sheets with the data
</commit_message>
<xml_diff>
--- a/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
+++ b/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>task-clock</t>
   </si>
@@ -102,9 +102,6 @@
     <t>[83.62%]</t>
   </si>
   <si>
-    <t>Lockless Single Producer Single Consumer Ring Buffer</t>
-  </si>
-  <si>
     <t>Stoker</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>Cube Lockless</t>
+  </si>
+  <si>
+    <t>Lockless Single Producer Single Consumer Ring Buffer for 3 sizes</t>
+  </si>
+  <si>
+    <t>PERF DATA BELOW</t>
   </si>
 </sst>
 </file>
@@ -478,11 +481,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97679616"/>
-        <c:axId val="40017920"/>
+        <c:axId val="96515584"/>
+        <c:axId val="114868608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97679616"/>
+        <c:axId val="96515584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40017920"/>
+        <c:crossAx val="114868608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -519,7 +522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40017920"/>
+        <c:axId val="114868608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +552,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97679616"/>
+        <c:crossAx val="96515584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1276,11 +1279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94040832"/>
-        <c:axId val="94042752"/>
+        <c:axId val="115218688"/>
+        <c:axId val="115241344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94040832"/>
+        <c:axId val="115218688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94042752"/>
+        <c:crossAx val="115241344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94042752"/>
+        <c:axId val="115241344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94040832"/>
+        <c:crossAx val="115218688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2082,11 +2085,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116049408"/>
-        <c:axId val="39145472"/>
+        <c:axId val="103037184"/>
+        <c:axId val="103051648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116049408"/>
+        <c:axId val="103037184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2115,7 +2118,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39145472"/>
+        <c:crossAx val="103051648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2123,7 +2126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39145472"/>
+        <c:axId val="103051648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,7 +2156,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116049408"/>
+        <c:crossAx val="103037184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2880,11 +2883,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105237504"/>
-        <c:axId val="105281792"/>
+        <c:axId val="103070336"/>
+        <c:axId val="103076608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105237504"/>
+        <c:axId val="103070336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2913,7 +2916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105281792"/>
+        <c:crossAx val="103076608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2921,7 +2924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105281792"/>
+        <c:axId val="103076608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +2954,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105237504"/>
+        <c:crossAx val="103070336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2978,13 +2981,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -3008,15 +3011,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
+      <xdr:colOff>552451</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>552451</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3038,15 +3041,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
+      <xdr:colOff>523876</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>219076</xdr:colOff>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3070,15 +3073,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
+      <xdr:colOff>485776</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>228601</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3391,8 +3394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3407,7 +3410,7 @@
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3423,7 +3426,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4">
         <v>7755224</v>
@@ -3437,7 +3440,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
         <v>8242413</v>
@@ -3451,7 +3454,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="5">
         <v>7575608</v>
@@ -3507,7 +3510,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4">
         <v>6558774</v>
@@ -3536,7 +3539,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4">
         <v>5642544</v>
@@ -3565,7 +3568,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4">
         <v>6163242</v>
@@ -3594,7 +3597,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="4">
         <v>4747505</v>
@@ -3623,7 +3626,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="4">
         <v>4910844</v>
@@ -3652,7 +3655,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="4">
         <v>4531949</v>
@@ -3681,7 +3684,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4">
         <v>4235748</v>
@@ -3710,7 +3713,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4">
         <v>5328217</v>
@@ -3739,7 +3742,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4">
         <v>9771618</v>
@@ -3768,7 +3771,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4">
         <v>14077775</v>
@@ -3797,7 +3800,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4">
         <v>11034242</v>
@@ -3826,7 +3829,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="4">
         <v>10644755</v>
@@ -3855,7 +3858,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="4">
         <v>10532349</v>
@@ -3884,7 +3887,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="4">
         <v>10604337</v>
@@ -3913,7 +3916,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="4">
         <v>6813876</v>
@@ -3942,7 +3945,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4">
         <v>6003533</v>
@@ -3971,7 +3974,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="4">
         <v>7482005</v>
@@ -4000,7 +4003,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4">
         <v>6178469</v>
@@ -4029,7 +4032,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="4">
         <v>6255918</v>
@@ -4058,7 +4061,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="4">
         <v>5980937</v>
@@ -4087,7 +4090,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="4">
         <v>6101158</v>
@@ -4138,7 +4141,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="4">
         <v>9906727</v>
@@ -4167,7 +4170,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="4">
         <v>8458383</v>
@@ -4196,7 +4199,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="5">
         <v>6074674</v>
@@ -4246,7 +4249,9 @@
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -4258,7 +4263,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4349,7 +4354,7 @@
         <v>9</v>
       </c>
       <c r="G47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4401,7 +4406,7 @@
         <v>12</v>
       </c>
       <c r="I49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4447,7 +4452,7 @@
         <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4493,12 +4498,12 @@
         <v>21</v>
       </c>
       <c r="I53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4589,7 +4594,7 @@
         <v>9</v>
       </c>
       <c r="G60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -4615,7 +4620,7 @@
         <v>12</v>
       </c>
       <c r="I61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -4641,7 +4646,7 @@
         <v>12</v>
       </c>
       <c r="I62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -4687,7 +4692,7 @@
         <v>20</v>
       </c>
       <c r="H64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
@@ -4707,7 +4712,7 @@
         <v>5</v>
       </c>
       <c r="G65" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
@@ -4733,7 +4738,7 @@
         <v>21</v>
       </c>
       <c r="I66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed the name of some files to better represent what is in them
</commit_message>
<xml_diff>
--- a/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
+++ b/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
   <si>
     <t>task-clock</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>PERF DATA BELOW</t>
+  </si>
+  <si>
+    <t>DATA IMPORTED FROM ring.cpp</t>
   </si>
 </sst>
 </file>
@@ -481,11 +484,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96515584"/>
-        <c:axId val="114868608"/>
+        <c:axId val="105383040"/>
+        <c:axId val="105384960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96515584"/>
+        <c:axId val="105383040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,7 +517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114868608"/>
+        <c:crossAx val="105384960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -522,7 +525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114868608"/>
+        <c:axId val="105384960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,7 +555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96515584"/>
+        <c:crossAx val="105383040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1279,11 +1282,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115218688"/>
-        <c:axId val="115241344"/>
+        <c:axId val="107287680"/>
+        <c:axId val="107289600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115218688"/>
+        <c:axId val="107287680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115241344"/>
+        <c:crossAx val="107289600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1320,7 +1323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115241344"/>
+        <c:axId val="107289600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115218688"/>
+        <c:crossAx val="107287680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2085,11 +2088,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103037184"/>
-        <c:axId val="103051648"/>
+        <c:axId val="107345024"/>
+        <c:axId val="107346944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103037184"/>
+        <c:axId val="107345024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2118,7 +2121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103051648"/>
+        <c:crossAx val="107346944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2126,7 +2129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103051648"/>
+        <c:axId val="107346944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103037184"/>
+        <c:crossAx val="107345024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2883,11 +2886,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103070336"/>
-        <c:axId val="103076608"/>
+        <c:axId val="107402752"/>
+        <c:axId val="107404672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103070336"/>
+        <c:axId val="107402752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,7 +2919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103076608"/>
+        <c:crossAx val="107404672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2924,7 +2927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103076608"/>
+        <c:axId val="107404672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2954,7 +2957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103070336"/>
+        <c:crossAx val="107402752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3395,12 +3398,12 @@
   <dimension ref="A5:O133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="1" max="1" width="57.140625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
@@ -3472,7 +3475,9 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>

</xml_diff>

<commit_message>
Added to the report, added data tables for all variations of the hash table and updated the presentation
</commit_message>
<xml_diff>
--- a/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
+++ b/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
@@ -418,11 +418,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100074624"/>
-        <c:axId val="100076544"/>
+        <c:axId val="40514688"/>
+        <c:axId val="40516608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100074624"/>
+        <c:axId val="40514688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,7 +451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100076544"/>
+        <c:crossAx val="40516608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -459,7 +459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100076544"/>
+        <c:axId val="40516608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100074624"/>
+        <c:crossAx val="40514688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1216,11 +1216,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101786752"/>
-        <c:axId val="101788672"/>
+        <c:axId val="40842368"/>
+        <c:axId val="40844288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101786752"/>
+        <c:axId val="40842368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1249,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101788672"/>
+        <c:crossAx val="40844288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1257,7 +1257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101788672"/>
+        <c:axId val="40844288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +1287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101786752"/>
+        <c:crossAx val="40842368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2022,11 +2022,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101840000"/>
-        <c:axId val="101841920"/>
+        <c:axId val="40907904"/>
+        <c:axId val="40909824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101840000"/>
+        <c:axId val="40907904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2055,7 +2055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101841920"/>
+        <c:crossAx val="40909824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2063,7 +2063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101841920"/>
+        <c:axId val="40909824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2093,7 +2093,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101840000"/>
+        <c:crossAx val="40907904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2820,11 +2820,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101897728"/>
-        <c:axId val="101899648"/>
+        <c:axId val="40953344"/>
+        <c:axId val="40955264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101897728"/>
+        <c:axId val="40953344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +2853,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101899648"/>
+        <c:crossAx val="40955264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2861,7 +2861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101899648"/>
+        <c:axId val="40955264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2891,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101897728"/>
+        <c:crossAx val="40953344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2947,16 +2947,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552451</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2978,15 +2978,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>523876</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3010,15 +3010,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>485776</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3331,7 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added to the report, updated the work diary
</commit_message>
<xml_diff>
--- a/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
+++ b/Data Structures/Single_Producer_Single_Consumer_Ring_Buffer/SPSC_Ring_Buffer.xlsx
@@ -418,11 +418,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40514688"/>
-        <c:axId val="40516608"/>
+        <c:axId val="97207424"/>
+        <c:axId val="97209344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40514688"/>
+        <c:axId val="97207424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,7 +451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40516608"/>
+        <c:crossAx val="97209344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -459,7 +459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40516608"/>
+        <c:axId val="97209344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40514688"/>
+        <c:crossAx val="97207424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1129,11 +1129,11 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$35</c:f>
+              <c:f>Sheet1!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Stoker Lockless</c:v>
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Locked</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1173,6 +1173,1154 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>Sheet1!$B$19:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5328217</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>418741</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>473308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>461109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>448645</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>432057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) CAS lock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9771618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9735489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9905043</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9916571</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9639092</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9802904</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9930743</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9515278</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Ticket</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>14077775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2235</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1364</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2618</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) TAS </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>11034242</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11705109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11760762</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11697060</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11760174</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11739005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11745876</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11074532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) TAS No Pause</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10644755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8292727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4840726</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4499906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4600061</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4661298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4934930</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4789439</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) TTAS No Pause</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10532349</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8121657</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5199081</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5238513</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4510888</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5273445</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4697164</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5243731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$25:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10604337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10611323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10564897</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10540146</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10570471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10592364</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10539685</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10488351</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E Cube ) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6813876</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13561445</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10716292</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9389905</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11458014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6445226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10594142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5268522</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E ) CAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6003533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7571208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5799059</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7543689</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5793887</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7527437</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6002122</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5780359</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E ) Ticket</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$28:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7482005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E ) TAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$29:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6178469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10791738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6209044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6032768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8061495</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6005502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8050999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6197390</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E ) TAS No Pause</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$30:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6255918</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9239428</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1671904</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1033345</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1092124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1006588</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>792270</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>194233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E ) TTAS No Pause</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$31:$I$31</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5980937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6756515</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10008867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6461166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7956106</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6155953</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1759228</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>239830</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="20"/>
+          <c:order val="20"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 Core Intel CPU @ 2.27 GHz (E ) TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6101158</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6096248</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6564101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6351205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6084325</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5934312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6006657</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6067944</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="21"/>
+          <c:order val="21"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Sheet1!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
@@ -1200,6 +2348,170 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9906727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="22"/>
+          <c:order val="22"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local Machine Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$I$36</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8458383</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8458383</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="23"/>
+          <c:order val="23"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cube Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6074674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6074674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,11 +2528,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40842368"/>
-        <c:axId val="40844288"/>
+        <c:axId val="98256000"/>
+        <c:axId val="98257920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40842368"/>
+        <c:axId val="98256000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +2561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40844288"/>
+        <c:crossAx val="98257920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1257,7 +2569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40844288"/>
+        <c:axId val="98257920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +2599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40842368"/>
+        <c:crossAx val="98256000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2022,11 +3334,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40907904"/>
-        <c:axId val="40909824"/>
+        <c:axId val="100152448"/>
+        <c:axId val="100154368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40907904"/>
+        <c:axId val="100152448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2055,7 +3367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40909824"/>
+        <c:crossAx val="100154368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2063,7 +3375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40909824"/>
+        <c:axId val="100154368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2093,7 +3405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40907904"/>
+        <c:crossAx val="100152448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2820,11 +4132,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40953344"/>
-        <c:axId val="40955264"/>
+        <c:axId val="100201984"/>
+        <c:axId val="100203904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40953344"/>
+        <c:axId val="100201984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +4165,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40955264"/>
+        <c:crossAx val="100203904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2861,7 +4173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40955264"/>
+        <c:axId val="100203904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +4203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40953344"/>
+        <c:crossAx val="100201984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2947,16 +4259,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3331,8 +4643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>